<commit_message>
feat: add MUEEN layout and some refactoring.
</commit_message>
<xml_diff>
--- a/Gemasolar/parameters.xlsx
+++ b/Gemasolar/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sth\Desktop\2022年光热太阳能仿真与建模\太阳能镜场数据整理\Gemasolar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331E3611-E6D4-484A-B73A-9DA3B815ABA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C21460D-45E2-4DDC-A05E-09BA7A2B911B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -26,23 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="86">
-  <si>
-    <t>位置</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>经度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>海拔</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>年DNI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="87">
   <si>
     <t>Sunshape</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -52,10 +36,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>镜面形状</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>canting condition</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -240,18 +220,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>参数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>环绕太阳比</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>跟踪类型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Heliostat</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -268,107 +236,464 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>太阳</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>定日镜</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>接收器</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>纬度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>太阳影响模型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>数量</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>倾斜规则</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>焦距</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>宽</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>高</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>反射率</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>法向扰动标准差</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>聚焦点</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>镜场类型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>接收器类型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>半径</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>接收器高度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>参考</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>方位角-高度角跟踪</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>矩形边界聚焦型定日镜</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>轴上倾斜</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>定日镜斜距</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>对准接收器中点</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>环绕型镜场</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>圆柱形接收器</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>参数</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>值</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>参考</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>位置</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>位置</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>纬度</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>经度</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>海拔</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>太阳</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>年</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>DNI</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>太阳影响模型</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>环绕太阳比</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>定日镜</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>跟踪类型</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>方位角</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>高度角跟踪</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>数量</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>镜面形状</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>矩形边界聚焦型定日镜</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>倾斜规则</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>轴上倾斜</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>焦距</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>定日镜斜距</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>宽</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>高</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>反射率</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>法向扰动标准差</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>聚焦点</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>对准接收器中点</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>接收器</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>镜场类型</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>环绕型镜场</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>接收器类型</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>圆柱形接收器</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>半径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>接收器高度</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -376,7 +701,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -400,6 +725,33 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -421,7 +773,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -431,6 +783,16 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -714,7 +1076,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -726,295 +1088,295 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C8" s="1">
         <v>0.05</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C10" s="1">
         <v>2650</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C16" s="1">
         <v>0.93</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1034,307 +1396,308 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36E56D1C-CF4D-4FCA-A2A0-34606D159E38}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="39.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="39.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.6640625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="6"/>
+      <c r="B4" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="6"/>
+      <c r="B5" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="6"/>
+      <c r="B8" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="6"/>
+      <c r="B10" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="7">
+        <v>2650</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="6"/>
+      <c r="B11" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="6"/>
+      <c r="B12" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="6"/>
+      <c r="B13" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="6"/>
+      <c r="B14" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="6"/>
+      <c r="B15" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="6"/>
+      <c r="B16" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="7">
+        <v>0.93</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="6"/>
+      <c r="B17" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="C17" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="6"/>
+      <c r="B18" s="7" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C18" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="6"/>
+      <c r="B20" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="6"/>
+      <c r="B21" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="6"/>
+      <c r="B22" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="6"/>
+      <c r="B23" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="1">
-        <v>2650</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
-      <c r="B12" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C16" s="1">
-        <v>0.93</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-      <c r="B17" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-      <c r="B18" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="3"/>
-      <c r="B20" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
-      <c r="B21" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="3"/>
-      <c r="B22" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="3"/>
-      <c r="B23" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>44</v>
+      <c r="D23" s="7" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>41</v>
+      <c r="A25" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>42</v>
+      <c r="A26" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1346,5 +1709,6 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>